<commit_message>
no_causal_20k_scen2_sim_summ_tib re-run 1000 CIs/point0 fixed. Starting re-check of citation data as discordant results.
</commit_message>
<xml_diff>
--- a/MSc_Thesis/MSc_Thesis_Split/Data/Citations_Datasets/carreras-torres_role_2017.xlsx
+++ b/MSc_Thesis/MSc_Thesis_Split/Data/Citations_Datasets/carreras-torres_role_2017.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/4f99f7067dc2a9a5/Documents/R/Working Directory/Data_Science_MSc/Dissertation_Bayes_MR/MSc_Thesis/MSc_Thesis_Split/Data/Citations_Datasets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="8" documentId="8_{3EE3051F-89E5-4C43-909D-934B6854326A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FAEF452C-BF1B-4F81-B986-F18E01BD8B20}"/>
+  <xr:revisionPtr revIDLastSave="9" documentId="8_{3EE3051F-89E5-4C43-909D-934B6854326A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{08966C80-EE81-41AD-936F-3F6B7CCA0B3F}"/>
   <bookViews>
-    <workbookView xWindow="-90" yWindow="0" windowWidth="12980" windowHeight="15370" xr2:uid="{C66FB6DB-99C0-45C6-9200-BF530454AB21}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{C66FB6DB-99C0-45C6-9200-BF530454AB21}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1954,6 +1954,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2275,11 +2279,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1897F6A-B250-4E7D-91CB-E090A2D066BE}">
   <dimension ref="A1:Q560"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A519" workbookViewId="0">
-      <selection activeCell="J3" sqref="J3:J560"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="U6" sqref="U6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="9" max="9" width="12.36328125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="G1" t="s">

</xml_diff>

<commit_message>
All sims except no_causal_20k_scen_3 re run 1000, point0/causal report fixed.
</commit_message>
<xml_diff>
--- a/MSc_Thesis/MSc_Thesis_Split/Data/Citations_Datasets/carreras-torres_role_2017.xlsx
+++ b/MSc_Thesis/MSc_Thesis_Split/Data/Citations_Datasets/carreras-torres_role_2017.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/4f99f7067dc2a9a5/Documents/R/Working Directory/Data_Science_MSc/Dissertation_Bayes_MR/MSc_Thesis/MSc_Thesis_Split/Data/Citations_Datasets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="8" documentId="8_{3EE3051F-89E5-4C43-909D-934B6854326A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FAEF452C-BF1B-4F81-B986-F18E01BD8B20}"/>
+  <xr:revisionPtr revIDLastSave="9" documentId="8_{3EE3051F-89E5-4C43-909D-934B6854326A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{08966C80-EE81-41AD-936F-3F6B7CCA0B3F}"/>
   <bookViews>
-    <workbookView xWindow="-90" yWindow="0" windowWidth="12980" windowHeight="15370" xr2:uid="{C66FB6DB-99C0-45C6-9200-BF530454AB21}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{C66FB6DB-99C0-45C6-9200-BF530454AB21}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1954,6 +1954,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2275,11 +2279,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1897F6A-B250-4E7D-91CB-E090A2D066BE}">
   <dimension ref="A1:Q560"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A519" workbookViewId="0">
-      <selection activeCell="J3" sqref="J3:J560"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="U6" sqref="U6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="9" max="9" width="12.36328125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="G1" t="s">

</xml_diff>